<commit_message>
Finalize model and SHAP Values Graph
</commit_message>
<xml_diff>
--- a/rahim_ghani_predict/result-analysis/auto-sklearn.xlsx
+++ b/rahim_ghani_predict/result-analysis/auto-sklearn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\msc-project\from-github\dissertations-2021-info\rahim_ghani_predict\result-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA04EB7-4BF1-467C-9D6D-4C64FD8C47BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8908A2D-DEE9-49B7-BD8A-EEBE214AB22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B4B1EB9E-4A42-415B-A819-52F34DF66FB1}"/>
   </bookViews>
@@ -487,7 +487,7 @@
   <dimension ref="A2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>